<commit_message>
allow mesh file upload
</commit_message>
<xml_diff>
--- a/morphosource_batch_convert/sample_data/MSBIW_test.xlsx
+++ b/morphosource_batch_convert/sample_data/MSBIW_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="262">
   <si>
     <t>MorphoSource Field</t>
   </si>
@@ -22,315 +22,330 @@
     <t>Description</t>
   </si>
   <si>
+    <t>microCT volume and derivatives of UF-I-187802</t>
+  </si>
+  <si>
+    <t>microCT volume and derivatives of UF-I-187802_head</t>
+  </si>
+  <si>
+    <t>microCT volume and derivatives of UF-I-236194</t>
+  </si>
+  <si>
+    <t>microCT volume and derivatives of UF-I-236194_head</t>
+  </si>
+  <si>
+    <t>microCT volume and derivatives of UF-I-78923</t>
+  </si>
+  <si>
+    <t>Specimen record (e.g., "NHM-VP-12345")</t>
+  </si>
+  <si>
+    <t>ms_specimens.specimen_id</t>
+  </si>
+  <si>
+    <t>MorphoSource Identifier.  Unique identifier of specimen record in MorphoSource.  Available on specimen detail page.  If provided, media groups will be linked to existing specimen record and no additional specimen metadata needs to be provided.</t>
+  </si>
+  <si>
+    <t>ms_specimens.occurrence_id</t>
+  </si>
+  <si>
+    <t>Occurrence ID.  Unique Institutional identifier for the specimen.  Will be used to attempt to link record to iDigBio specimen</t>
+  </si>
+  <si>
+    <t>b6edc7cb-c80f-4484-afd0-d041e59f7afc</t>
+  </si>
+  <si>
+    <t>7b3af0b0-6e81-42c6-a3ee-fe6cb7be1407</t>
+  </si>
+  <si>
+    <t>c2a4eab9-fe5d-4336-8a86-2f15b5dc6b35</t>
+  </si>
+  <si>
+    <t>ms_specimens.institution_code</t>
+  </si>
+  <si>
+    <t>Institution code prefix  (e.g., "NHM-")</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>ms_specimens.collection_code</t>
+  </si>
+  <si>
+    <t>Collection code modifier (e.g., "VP-")</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>ms_specimens.catalog_number</t>
+  </si>
+  <si>
+    <t>Alphanumeric string  (e.g., "12345")</t>
+  </si>
+  <si>
+    <t>187802</t>
+  </si>
+  <si>
+    <t>236194</t>
+  </si>
+  <si>
+    <t>78923</t>
+  </si>
+  <si>
+    <t>ms_specimens.url</t>
+  </si>
+  <si>
+    <t>URL to specimen record in home repository</t>
+  </si>
+  <si>
+    <t>ms_specimens.reference_source</t>
+  </si>
+  <si>
+    <t>Reference Source</t>
+  </si>
+  <si>
+    <t>ms_specimens.collector</t>
+  </si>
+  <si>
+    <t>Who collected the specimen</t>
+  </si>
+  <si>
+    <t>ms_specimens.collected_on</t>
+  </si>
+  <si>
+    <t>Specimen collection date</t>
+  </si>
+  <si>
+    <t>ms_specimens.description</t>
+  </si>
+  <si>
+    <t>General description of specimen physical content</t>
+  </si>
+  <si>
+    <t>ms_specimens.type</t>
+  </si>
+  <si>
+    <t>Holotype</t>
+  </si>
+  <si>
+    <t>ms_specimens.sex</t>
+  </si>
+  <si>
+    <t>Sex of specimen</t>
+  </si>
+  <si>
+    <t>ms_specimens.notes</t>
+  </si>
+  <si>
+    <t>Notes about the specimen</t>
+  </si>
+  <si>
+    <t>ms_specimens.relative_age</t>
+  </si>
+  <si>
+    <t>Geologic Age</t>
+  </si>
+  <si>
+    <t>ms_specimens.absolute_age</t>
+  </si>
+  <si>
+    <t>Absolute age</t>
+  </si>
+  <si>
+    <t>ms_specimens.body_mass</t>
+  </si>
+  <si>
+    <t>Body mass</t>
+  </si>
+  <si>
+    <t>ms_specimens.body_mass_comments</t>
+  </si>
+  <si>
+    <t>Body mass comments</t>
+  </si>
+  <si>
+    <t>ms_specimens.locality_description</t>
+  </si>
+  <si>
+    <t>Verbatim locality</t>
+  </si>
+  <si>
+    <t>ms_specimens.locality_coordinates</t>
+  </si>
+  <si>
+    <t>Type of coordinates of the locality of the specimen</t>
+  </si>
+  <si>
+    <t>ms_specimens.locality_datum_zone</t>
+  </si>
+  <si>
+    <t>Locality datum/zone</t>
+  </si>
+  <si>
+    <t>ms_specimens.locality_northing_coordinate</t>
+  </si>
+  <si>
+    <t>Locality northing coordinate</t>
+  </si>
+  <si>
+    <t>ms_specimens.locality_easting_coordinate</t>
+  </si>
+  <si>
+    <t>Locality easting coordinate</t>
+  </si>
+  <si>
+    <t>ms_specimens.locality_absolute_age</t>
+  </si>
+  <si>
+    <t>Locality absolute age</t>
+  </si>
+  <si>
+    <t>ms_specimens.locality_relative_age</t>
+  </si>
+  <si>
+    <t>Locality geologic age</t>
+  </si>
+  <si>
+    <t>ms_taxonomy.common_name</t>
+  </si>
+  <si>
+    <t>Common name for taxon</t>
+  </si>
+  <si>
+    <t>ms_taxonomy.is_extinct</t>
+  </si>
+  <si>
+    <t>Is taxa extinct?</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.genus</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.species</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.subspecies</t>
+  </si>
+  <si>
+    <t>Subspecies</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.variety</t>
+  </si>
+  <si>
+    <t>Variety</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.author</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.year</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_supraspecific_clade</t>
+  </si>
+  <si>
+    <t>Higher ss. Clade</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_kingdom</t>
+  </si>
+  <si>
+    <t>Higher kingdom</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_phylum</t>
+  </si>
+  <si>
+    <t>Higher Phylum</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_class</t>
+  </si>
+  <si>
+    <t>Higher class</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_subclass</t>
+  </si>
+  <si>
+    <t>Higher subclass</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_superorder</t>
+  </si>
+  <si>
+    <t>Higher superorder</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_order</t>
+  </si>
+  <si>
+    <t>Higher order</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_suborder</t>
+  </si>
+  <si>
+    <t>Higher suborder</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_superfamily</t>
+  </si>
+  <si>
+    <t>Higher superfamily</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_family</t>
+  </si>
+  <si>
+    <t>Higher family</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.ht_subfamily</t>
+  </si>
+  <si>
+    <t>Higher subfamily</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.source_info</t>
+  </si>
+  <si>
+    <t>Source Information</t>
+  </si>
+  <si>
+    <t>ms_taxonomy_names.notes</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Media Group (e.g., grouping of a Ct volume and a derivative mesh file created from it)</t>
+  </si>
+  <si>
+    <t>ms_media.title</t>
+  </si>
+  <si>
+    <t>Optional description of media group</t>
+  </si>
+  <si>
     <t>microCT volume and derivatives</t>
   </si>
   <si>
-    <t>Specimen record (e.g., "NHM-VP-12345")</t>
-  </si>
-  <si>
-    <t>ms_specimens.specimen_id</t>
-  </si>
-  <si>
-    <t>MorphoSource Identifier.  Unique identifier of specimen record in MorphoSource.  Available on specimen detail page.  If provided, media groups will be linked to existing specimen record and no additional specimen metadata needs to be provided.</t>
-  </si>
-  <si>
-    <t>ms_specimens.occurrence_id</t>
-  </si>
-  <si>
-    <t>Occurrence ID.  Unique Institutional identifier for the specimen.  Will be used to attempt to link record to iDigBio specimen</t>
-  </si>
-  <si>
-    <t>b6edc7cb-c80f-4484-afd0-d041e59f7afc</t>
-  </si>
-  <si>
-    <t>7b3af0b0-6e81-42c6-a3ee-fe6cb7be1407</t>
-  </si>
-  <si>
-    <t>c2a4eab9-fe5d-4336-8a86-2f15b5dc6b35</t>
-  </si>
-  <si>
-    <t>ms_specimens.institution_code</t>
-  </si>
-  <si>
-    <t>Institution code prefix  (e.g., "NHM-")</t>
-  </si>
-  <si>
-    <t>UF</t>
-  </si>
-  <si>
-    <t>ms_specimens.collection_code</t>
-  </si>
-  <si>
-    <t>Collection code modifier (e.g., "VP-")</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-  <si>
-    <t>ms_specimens.catalog_number</t>
-  </si>
-  <si>
-    <t>Alphanumeric string  (e.g., "12345")</t>
-  </si>
-  <si>
-    <t>187802</t>
-  </si>
-  <si>
-    <t>236194</t>
-  </si>
-  <si>
-    <t>78923</t>
-  </si>
-  <si>
-    <t>ms_specimens.url</t>
-  </si>
-  <si>
-    <t>URL to specimen record in home repository</t>
-  </si>
-  <si>
-    <t>ms_specimens.reference_source</t>
-  </si>
-  <si>
-    <t>Reference Source</t>
-  </si>
-  <si>
-    <t>ms_specimens.collector</t>
-  </si>
-  <si>
-    <t>Who collected the specimen</t>
-  </si>
-  <si>
-    <t>ms_specimens.collected_on</t>
-  </si>
-  <si>
-    <t>Specimen collection date</t>
-  </si>
-  <si>
-    <t>ms_specimens.description</t>
-  </si>
-  <si>
-    <t>General description of specimen physical content</t>
-  </si>
-  <si>
-    <t>ms_specimens.type</t>
-  </si>
-  <si>
-    <t>Holotype</t>
-  </si>
-  <si>
-    <t>ms_specimens.sex</t>
-  </si>
-  <si>
-    <t>Sex of specimen</t>
-  </si>
-  <si>
-    <t>ms_specimens.notes</t>
-  </si>
-  <si>
-    <t>Notes about the specimen</t>
-  </si>
-  <si>
-    <t>ms_specimens.relative_age</t>
-  </si>
-  <si>
-    <t>Geologic Age</t>
-  </si>
-  <si>
-    <t>ms_specimens.absolute_age</t>
-  </si>
-  <si>
-    <t>Absolute age</t>
-  </si>
-  <si>
-    <t>ms_specimens.body_mass</t>
-  </si>
-  <si>
-    <t>Body mass</t>
-  </si>
-  <si>
-    <t>ms_specimens.body_mass_comments</t>
-  </si>
-  <si>
-    <t>Body mass comments</t>
-  </si>
-  <si>
-    <t>ms_specimens.locality_description</t>
-  </si>
-  <si>
-    <t>Verbatim locality</t>
-  </si>
-  <si>
-    <t>ms_specimens.locality_coordinates</t>
-  </si>
-  <si>
-    <t>Type of coordinates of the locality of the specimen</t>
-  </si>
-  <si>
-    <t>ms_specimens.locality_datum_zone</t>
-  </si>
-  <si>
-    <t>Locality datum/zone</t>
-  </si>
-  <si>
-    <t>ms_specimens.locality_northing_coordinate</t>
-  </si>
-  <si>
-    <t>Locality northing coordinate</t>
-  </si>
-  <si>
-    <t>ms_specimens.locality_easting_coordinate</t>
-  </si>
-  <si>
-    <t>Locality easting coordinate</t>
-  </si>
-  <si>
-    <t>ms_specimens.locality_absolute_age</t>
-  </si>
-  <si>
-    <t>Locality absolute age</t>
-  </si>
-  <si>
-    <t>ms_specimens.locality_relative_age</t>
-  </si>
-  <si>
-    <t>Locality geologic age</t>
-  </si>
-  <si>
-    <t>ms_taxonomy.common_name</t>
-  </si>
-  <si>
-    <t>Common name for taxon</t>
-  </si>
-  <si>
-    <t>ms_taxonomy.is_extinct</t>
-  </si>
-  <si>
-    <t>Is taxa extinct?</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.genus</t>
-  </si>
-  <si>
-    <t>Genus</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.species</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.subspecies</t>
-  </si>
-  <si>
-    <t>Subspecies</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.variety</t>
-  </si>
-  <si>
-    <t>Variety</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.author</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.year</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_supraspecific_clade</t>
-  </si>
-  <si>
-    <t>Higher ss. Clade</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_kingdom</t>
-  </si>
-  <si>
-    <t>Higher kingdom</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_phylum</t>
-  </si>
-  <si>
-    <t>Higher Phylum</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_class</t>
-  </si>
-  <si>
-    <t>Higher class</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_subclass</t>
-  </si>
-  <si>
-    <t>Higher subclass</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_superorder</t>
-  </si>
-  <si>
-    <t>Higher superorder</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_order</t>
-  </si>
-  <si>
-    <t>Higher order</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_suborder</t>
-  </si>
-  <si>
-    <t>Higher suborder</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_superfamily</t>
-  </si>
-  <si>
-    <t>Higher superfamily</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_family</t>
-  </si>
-  <si>
-    <t>Higher family</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.ht_subfamily</t>
-  </si>
-  <si>
-    <t>Higher subfamily</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.source_info</t>
-  </si>
-  <si>
-    <t>Source Information</t>
-  </si>
-  <si>
-    <t>ms_taxonomy_names.notes</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Media Group (e.g., grouping of a Ct volume and a derivative mesh file created from it)</t>
-  </si>
-  <si>
-    <t>ms_media.title</t>
-  </si>
-  <si>
-    <t>Optional description of media group</t>
-  </si>
-  <si>
     <t>ms_media.published</t>
   </si>
   <si>
@@ -604,6 +619,9 @@
     <t>Optional display title for image</t>
   </si>
   <si>
+    <t>zipped tiff stack</t>
+  </si>
+  <si>
     <t>ms_media_files.element.1</t>
   </si>
   <si>
@@ -646,12 +664,27 @@
     <t>ms_media_files.media.2</t>
   </si>
   <si>
+    <t>UF-I-187802_raw.stl</t>
+  </si>
+  <si>
+    <t>UF-I-78923_cropped.ply</t>
+  </si>
+  <si>
     <t>ms_media_files.media_preview.2</t>
   </si>
   <si>
+    <t>UF-I-78923_cropped.png</t>
+  </si>
+  <si>
     <t>ms_media_files.title.2</t>
   </si>
   <si>
+    <t>raw mesh file</t>
+  </si>
+  <si>
+    <t>cropped mesh file</t>
+  </si>
+  <si>
     <t>ms_media_files.element.2</t>
   </si>
   <si>
@@ -664,6 +697,9 @@
     <t>ms_media_files.file_type.2</t>
   </si>
   <si>
+    <t>derivative</t>
+  </si>
+  <si>
     <t>ms_media_files.notes.2</t>
   </si>
   <si>
@@ -676,7 +712,13 @@
     <t>ms_media_files.media.3</t>
   </si>
   <si>
+    <t>UF-I-78923_raw.ply</t>
+  </si>
+  <si>
     <t>ms_media_files.media_preview.3</t>
+  </si>
+  <si>
+    <t>UF-I-78923_raw.png</t>
   </si>
   <si>
     <t>ms_media_files.title.3</t>
@@ -1097,25 +1139,25 @@
   <sheetData>
     <row r="1" spans="1:120">
       <c r="B1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AU1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="BX1" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="CG1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="CP1" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="CY1" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="DH1" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:120">
@@ -1123,361 +1165,361 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="S2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="T2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="U2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="V2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="W2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="X2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Y2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="Z2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AA2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AB2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AC2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="AD2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AE2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AF2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AG2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AH2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AI2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AJ2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AK2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AL2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="AM2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AN2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="AO2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="AP2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="AQ2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="AR2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="AS2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AT2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AU2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AV2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="AW2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="AX2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="AY2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="AZ2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="BA2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="BB2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="BC2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="BD2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="BE2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="BF2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="BG2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="BH2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="BI2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="BJ2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="BK2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="BL2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="BM2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="BN2" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="BO2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="BP2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="BQ2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="BR2" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="BS2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="BT2" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="BU2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="BV2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="BW2" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="BX2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="BY2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="BZ2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="CA2" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="CB2" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="CC2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="CD2" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="CE2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="CF2" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="CG2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="CH2" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="CI2" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="CJ2" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="CK2" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="CL2" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="CM2" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="CN2" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="CO2" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="CP2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="CQ2" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="CR2" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="CS2" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="CT2" t="s">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="CU2" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="CV2" t="s">
-        <v>225</v>
+        <v>239</v>
       </c>
       <c r="CW2" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="CX2" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="CY2" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="CZ2" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="DA2" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="DB2" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="DC2" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="DD2" t="s">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="DE2" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="DF2" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="DG2" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="DH2" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="DI2" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="DJ2" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="DK2" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="DL2" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="DM2" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="DN2" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="DO2" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="DP2" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:120">
@@ -1485,361 +1527,361 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="O3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="P3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="Q3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="R3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="S3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="T3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="U3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="V3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="W3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="X3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Y3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="Z3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AA3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AC3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AD3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AE3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AF3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AG3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AH3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AI3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AK3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="AL3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AM3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="AN3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="AO3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="AP3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="AQ3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="AR3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="AS3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AT3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="AU3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="AV3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="AW3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="AX3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="AY3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="AZ3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="BA3" t="s">
+        <v>125</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>135</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG3" t="s">
+        <v>141</v>
+      </c>
+      <c r="BH3" t="s">
+        <v>144</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>149</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>151</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>153</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>156</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>161</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>163</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>165</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>169</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>177</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>179</v>
+      </c>
+      <c r="BT3" t="s">
+        <v>181</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>183</v>
+      </c>
+      <c r="BV3" t="s">
+        <v>185</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>187</v>
+      </c>
+      <c r="BX3" t="s">
+        <v>191</v>
+      </c>
+      <c r="BY3" t="s">
+        <v>198</v>
+      </c>
+      <c r="BZ3" t="s">
+        <v>200</v>
+      </c>
+      <c r="CA3" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB3" t="s">
+        <v>205</v>
+      </c>
+      <c r="CC3" t="s">
+        <v>207</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>209</v>
+      </c>
+      <c r="CE3" t="s">
         <v>120</v>
       </c>
-      <c r="BB3" t="s">
-        <v>123</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>125</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>128</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>130</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>133</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>136</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>139</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>144</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>146</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>148</v>
-      </c>
-      <c r="BL3" t="s">
-        <v>151</v>
-      </c>
-      <c r="BM3" t="s">
-        <v>156</v>
-      </c>
-      <c r="BN3" t="s">
-        <v>158</v>
-      </c>
-      <c r="BO3" t="s">
-        <v>160</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>164</v>
-      </c>
-      <c r="BQ3" t="s">
-        <v>169</v>
-      </c>
-      <c r="BR3" t="s">
-        <v>172</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>174</v>
-      </c>
-      <c r="BT3" t="s">
-        <v>176</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>178</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>180</v>
-      </c>
-      <c r="BW3" t="s">
-        <v>182</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>186</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>193</v>
-      </c>
-      <c r="BZ3" t="s">
-        <v>195</v>
-      </c>
-      <c r="CA3" t="s">
-        <v>197</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>199</v>
-      </c>
-      <c r="CC3" t="s">
-        <v>201</v>
-      </c>
-      <c r="CD3" t="s">
+      <c r="CF3" t="s">
+        <v>213</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>191</v>
+      </c>
+      <c r="CH3" t="s">
+        <v>198</v>
+      </c>
+      <c r="CI3" t="s">
+        <v>200</v>
+      </c>
+      <c r="CJ3" t="s">
         <v>203</v>
       </c>
-      <c r="CE3" t="s">
-        <v>115</v>
-      </c>
-      <c r="CF3" t="s">
+      <c r="CK3" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL3" t="s">
         <v>207</v>
       </c>
-      <c r="CG3" t="s">
-        <v>186</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CI3" t="s">
-        <v>195</v>
-      </c>
-      <c r="CJ3" t="s">
-        <v>197</v>
-      </c>
-      <c r="CK3" t="s">
-        <v>199</v>
-      </c>
-      <c r="CL3" t="s">
-        <v>201</v>
-      </c>
       <c r="CM3" t="s">
+        <v>209</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>120</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>213</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>191</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>198</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>200</v>
+      </c>
+      <c r="CS3" t="s">
         <v>203</v>
       </c>
-      <c r="CN3" t="s">
-        <v>115</v>
-      </c>
-      <c r="CO3" t="s">
+      <c r="CT3" t="s">
+        <v>205</v>
+      </c>
+      <c r="CU3" t="s">
         <v>207</v>
       </c>
-      <c r="CP3" t="s">
-        <v>186</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>193</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>195</v>
-      </c>
-      <c r="CS3" t="s">
-        <v>197</v>
-      </c>
-      <c r="CT3" t="s">
-        <v>199</v>
-      </c>
-      <c r="CU3" t="s">
-        <v>201</v>
-      </c>
       <c r="CV3" t="s">
+        <v>209</v>
+      </c>
+      <c r="CW3" t="s">
+        <v>120</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>213</v>
+      </c>
+      <c r="CY3" t="s">
+        <v>191</v>
+      </c>
+      <c r="CZ3" t="s">
+        <v>198</v>
+      </c>
+      <c r="DA3" t="s">
+        <v>200</v>
+      </c>
+      <c r="DB3" t="s">
         <v>203</v>
       </c>
-      <c r="CW3" t="s">
-        <v>115</v>
-      </c>
-      <c r="CX3" t="s">
+      <c r="DC3" t="s">
+        <v>205</v>
+      </c>
+      <c r="DD3" t="s">
         <v>207</v>
       </c>
-      <c r="CY3" t="s">
-        <v>186</v>
-      </c>
-      <c r="CZ3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DA3" t="s">
-        <v>195</v>
-      </c>
-      <c r="DB3" t="s">
-        <v>197</v>
-      </c>
-      <c r="DC3" t="s">
-        <v>199</v>
-      </c>
-      <c r="DD3" t="s">
-        <v>201</v>
-      </c>
       <c r="DE3" t="s">
+        <v>209</v>
+      </c>
+      <c r="DF3" t="s">
+        <v>120</v>
+      </c>
+      <c r="DG3" t="s">
+        <v>213</v>
+      </c>
+      <c r="DH3" t="s">
+        <v>191</v>
+      </c>
+      <c r="DI3" t="s">
+        <v>198</v>
+      </c>
+      <c r="DJ3" t="s">
+        <v>200</v>
+      </c>
+      <c r="DK3" t="s">
         <v>203</v>
       </c>
-      <c r="DF3" t="s">
-        <v>115</v>
-      </c>
-      <c r="DG3" t="s">
+      <c r="DL3" t="s">
+        <v>205</v>
+      </c>
+      <c r="DM3" t="s">
         <v>207</v>
       </c>
-      <c r="DH3" t="s">
-        <v>186</v>
-      </c>
-      <c r="DI3" t="s">
-        <v>193</v>
-      </c>
-      <c r="DJ3" t="s">
-        <v>195</v>
-      </c>
-      <c r="DK3" t="s">
-        <v>197</v>
-      </c>
-      <c r="DL3" t="s">
-        <v>199</v>
-      </c>
-      <c r="DM3" t="s">
-        <v>201</v>
-      </c>
       <c r="DN3" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="DO3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="DP3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:120">
@@ -1847,61 +1889,61 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AU4" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="AW4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AX4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AZ4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="BA4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="BC4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="BD4" t="b">
         <v>1</v>
       </c>
       <c r="BE4" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="BF4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="BG4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="BH4" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BI4" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BJ4" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BK4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="BL4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="BM4">
         <v>13</v>
@@ -1910,13 +1952,13 @@
         <v>0.250097</v>
       </c>
       <c r="BO4" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="BP4" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="BQ4" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="BS4" t="b">
         <v>1</v>
@@ -1928,75 +1970,87 @@
         <v>0</v>
       </c>
       <c r="BW4" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="BX4" t="s">
-        <v>187</v>
+        <v>192</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>201</v>
       </c>
       <c r="CD4" t="s">
-        <v>204</v>
+        <v>210</v>
+      </c>
+      <c r="CG4" t="s">
+        <v>216</v>
+      </c>
+      <c r="CI4" t="s">
+        <v>221</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:120">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AU5" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="AW5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AX5" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AZ5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="BA5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="BC5" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="BD5" t="b">
         <v>1</v>
       </c>
       <c r="BE5" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="BF5" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="BG5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="BH5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BI5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BJ5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BK5" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="BL5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="BM5">
         <v>13</v>
@@ -2005,13 +2059,13 @@
         <v>0.250097</v>
       </c>
       <c r="BO5" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="BP5" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="BQ5" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="BS5" t="b">
         <v>1</v>
@@ -2023,75 +2077,78 @@
         <v>0</v>
       </c>
       <c r="BW5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="BX5" t="s">
-        <v>188</v>
+        <v>193</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>201</v>
       </c>
       <c r="CD5" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:120">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AU6" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="AW6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AX6" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AZ6" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="BA6" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="BC6" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="BD6" t="b">
         <v>1</v>
       </c>
       <c r="BE6" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="BF6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="BG6" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="BH6" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BI6" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BJ6" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="BK6" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="BL6" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="BM6">
         <v>13</v>
@@ -2100,13 +2157,13 @@
         <v>0.250097</v>
       </c>
       <c r="BO6" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="BP6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="BQ6" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="BS6" t="b">
         <v>1</v>
@@ -2118,75 +2175,78 @@
         <v>0</v>
       </c>
       <c r="BW6" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="BX6" t="s">
-        <v>189</v>
+        <v>194</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>201</v>
       </c>
       <c r="CD6" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:120">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AU7" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="AW7" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AX7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AZ7" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="BA7" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="BC7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="BD7" t="b">
         <v>1</v>
       </c>
       <c r="BE7" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="BF7" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="BG7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="BH7" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="BI7" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="BJ7" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="BK7" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="BL7" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="BM7">
         <v>15</v>
@@ -2195,13 +2255,13 @@
         <v>0.200098</v>
       </c>
       <c r="BO7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="BP7" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="BQ7" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="BS7" t="b">
         <v>1</v>
@@ -2213,75 +2273,78 @@
         <v>0</v>
       </c>
       <c r="BW7" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="BX7" t="s">
-        <v>190</v>
+        <v>195</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>201</v>
       </c>
       <c r="CD7" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:120">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AU8" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="AW8" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="AX8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AZ8" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="BA8" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="BC8" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="BD8" t="b">
         <v>1</v>
       </c>
       <c r="BE8" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="BF8" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="BG8" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="BH8" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="BI8" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="BJ8" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="BK8" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="BL8" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="BM8">
         <v>6</v>
@@ -2290,13 +2353,13 @@
         <v>0.333096</v>
       </c>
       <c r="BO8" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="BP8" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="BQ8" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="BS8" t="b">
         <v>1</v>
@@ -2308,13 +2371,40 @@
         <v>0</v>
       </c>
       <c r="BW8" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="BX8" t="s">
-        <v>191</v>
+        <v>196</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>201</v>
       </c>
       <c r="CD8" t="s">
-        <v>204</v>
+        <v>210</v>
+      </c>
+      <c r="CG8" t="s">
+        <v>217</v>
+      </c>
+      <c r="CH8" t="s">
+        <v>219</v>
+      </c>
+      <c r="CI8" t="s">
+        <v>222</v>
+      </c>
+      <c r="CM8" t="s">
+        <v>227</v>
+      </c>
+      <c r="CP8" t="s">
+        <v>232</v>
+      </c>
+      <c r="CQ8" t="s">
+        <v>234</v>
+      </c>
+      <c r="CR8" t="s">
+        <v>221</v>
+      </c>
+      <c r="CV8" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>